<commit_message>
updated LED resistor values, updated partlists, minor change to daughterboard template
</commit_message>
<xml_diff>
--- a/shields/probe_shield/partlist_probe_shield.xlsx
+++ b/shields/probe_shield/partlist_probe_shield.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\hive\shields\probe_shield\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA563F9-0D74-4920-A15A-79D49924A212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88EC4A0B-5B27-4834-AB33-76BECA7B4D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-870" yWindow="3195" windowWidth="2355" windowHeight="9045" xr2:uid="{4D41A2A2-8ED5-4738-9464-E3B21CDC951E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{4D41A2A2-8ED5-4738-9464-E3B21CDC951E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
-  <si>
-    <t>10u</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>-</t>
   </si>
@@ -108,9 +105,6 @@
     <t>Total CHF</t>
   </si>
   <si>
-    <t>&gt;  H1-H6</t>
-  </si>
-  <si>
     <t xml:space="preserve">    J4</t>
   </si>
   <si>
@@ -120,9 +114,6 @@
     <t xml:space="preserve">    J6</t>
   </si>
   <si>
-    <t>MountingHole</t>
-  </si>
-  <si>
     <t>Probe Channel 0</t>
   </si>
   <si>
@@ -139,6 +130,15 @@
   </si>
   <si>
     <t>TSW-113-07-L-D</t>
+  </si>
+  <si>
+    <t>Capacitor 10uF</t>
+  </si>
+  <si>
+    <t>CL21A106KPFNNNF</t>
+  </si>
+  <si>
+    <t>Resistor 0603 560Ohm</t>
   </si>
 </sst>
 </file>
@@ -196,19 +196,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -527,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DE50153-71A2-4622-BA68-B62B9D162F18}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,36 +540,39 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -583,10 +580,10 @@
       <c r="E2" s="2">
         <v>0.13</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>0.15</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <f>E2*D2</f>
         <v>0.26</v>
       </c>
@@ -597,59 +594,69 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.64</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3" si="0">E3*D3</f>
+        <v>0.64</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3" si="1">F3*D3</f>
+        <v>0.62</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" s="2">
-        <v>0.64</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0.62</v>
-      </c>
-      <c r="G4" s="4">
-        <f t="shared" ref="G4" si="0">E4*D4</f>
-        <v>0.64</v>
+        <v>3.61</v>
+      </c>
+      <c r="F4" s="3">
+        <v>3.56</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" ref="G4:G10" si="2">E4*D4</f>
+        <v>3.61</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4" si="1">F4*D4</f>
-        <v>0.62</v>
+        <f t="shared" ref="H4:H10" si="3">F4*D4</f>
+        <v>3.56</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -657,27 +664,27 @@
       <c r="E5" s="2">
         <v>3.61</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>3.56</v>
       </c>
-      <c r="G5" s="4">
-        <f t="shared" ref="G5:G11" si="2">E5*D5</f>
+      <c r="G5" s="3">
+        <f t="shared" si="2"/>
         <v>3.61</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H11" si="3">F5*D5</f>
+        <f t="shared" si="3"/>
         <v>3.56</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
         <v>30</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -685,10 +692,10 @@
       <c r="E6" s="2">
         <v>3.61</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>3.56</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <f t="shared" si="2"/>
         <v>3.61</v>
       </c>
@@ -699,13 +706,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -713,10 +720,10 @@
       <c r="E7" s="2">
         <v>3.61</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>3.56</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <f t="shared" si="2"/>
         <v>3.61</v>
       </c>
@@ -727,149 +734,121 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" s="2">
-        <v>3.61</v>
-      </c>
-      <c r="F8" s="4">
-        <v>3.56</v>
-      </c>
-      <c r="G8" s="4">
+        <v>2.77</v>
+      </c>
+      <c r="F8" s="3">
+        <v>2.74</v>
+      </c>
+      <c r="G8" s="3">
         <f t="shared" si="2"/>
-        <v>3.61</v>
+        <v>2.77</v>
       </c>
       <c r="H8">
         <f t="shared" si="3"/>
-        <v>3.56</v>
+        <v>2.74</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" s="2">
-        <v>2.77</v>
-      </c>
-      <c r="F9" s="4">
-        <v>2.74</v>
-      </c>
-      <c r="G9" s="4">
+        <v>2.02</v>
+      </c>
+      <c r="F9" s="3">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="G9" s="3">
         <f t="shared" si="2"/>
-        <v>2.77</v>
+        <v>2.02</v>
       </c>
       <c r="H9">
         <f t="shared" si="3"/>
-        <v>2.74</v>
+        <v>2.0099999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" s="2">
-        <v>2.02</v>
-      </c>
-      <c r="F10" s="4">
-        <v>2.0099999999999998</v>
-      </c>
-      <c r="G10" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G10" s="3">
         <f t="shared" si="2"/>
-        <v>2.02</v>
+        <v>0.13</v>
       </c>
       <c r="H10">
         <f t="shared" si="3"/>
-        <v>2.0099999999999998</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
-      <c r="E11" s="2">
-        <v>0.13</v>
-      </c>
-      <c r="F11" s="4">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="G11" s="4">
-        <f t="shared" si="2"/>
-        <v>0.13</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="3"/>
-        <v>0.14000000000000001</v>
-      </c>
+      <c r="E11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12">
-        <v>195</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G12" s="4"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E13" s="2"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F14" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="7">
-        <f>SUM(G2:G13)</f>
+      <c r="F13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="5">
+        <f>SUM(G2:G12)</f>
         <v>20.259999999999998</v>
       </c>
-      <c r="H14" s="7">
-        <f>SUM(H2:H13)</f>
+      <c r="H13" s="5">
+        <f>SUM(H2:H12)</f>
         <v>20.050000000000004</v>
       </c>
     </row>

</xml_diff>